<commit_message>
Update documentation and remove obsolete example
- Updated Dokumentation.xlsx with latest changes
- Removed SimpleServoTest example (no longer needed)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Dokumentation.xlsx
+++ b/Dokumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasschoning/Documents/Arduino/libraries/BuggyControl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF5425F-4009-7942-AAD1-F04B3EA5477F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01A3C4-1CBD-D34A-85D4-BDBBB5ED6DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{485CC123-1C10-6045-B34C-C7CEBDC1B1A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{485CC123-1C10-6045-B34C-C7CEBDC1B1A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Dokumentation BuggyControl Library
 -Niklas Schöning</t>
@@ -72,22 +72,6 @@
 setzt die Motor-Duty sofort auf target_duty</t>
   </si>
   <si>
-    <t>private void fadeDuty(
-int target_duty
-)
-nähert Motor-Duty über ledcFade-Funktion linear target_duty an</t>
-  </si>
-  <si>
-    <t>private void safetyDelay(
-)
-blocking Delay mit direction_change_delay Dauer, setzt alle Pins auf 0 Spannung bzw. Duty</t>
-  </si>
-  <si>
-    <t>private void startDelay(
-)
-Non-blocking Delay starten, welches die changeSpeedFunktion blockiert. Setzt alle Pins auf 0 Spannung oder Duty</t>
-  </si>
-  <si>
     <t>public int getCurrentDuty(
 )
 gibt current_duty zurück</t>
@@ -140,70 +124,105 @@
 schaltet LEDs an mit Helligkeit _brightness in %</t>
   </si>
   <si>
+    <t>public void turnOff(
+)
+schaltet alle LEDs aus</t>
+  </si>
+  <si>
+    <t>private int percentToDegree(
+int steering_percent
+)
+gibt steering_percent in Grad umgewandelt zurück</t>
+  </si>
+  <si>
+    <t>public int getSteeringDegree(
+)
+Gibt aktuellen Lenkwinkeln zurück</t>
+  </si>
+  <si>
+    <t>public void changeSpeed(
+int direction_vector 
+)
+Diese Funktion sollte zum Ändern der Motorgeschwindigkeit als einzige direkt aufgerufen wird. Direction_vector ist die erwünschte Veränderung des Duty-Cycles/der Geschwindigkeit in %, kein absoluter Wert. Entscheidet anhand von threshhold, ob fadeDuty oder setDuty genutzt werden soll, initialisiert safetyDelay bei Richtungswechsel oder anhalten u.w.</t>
+  </si>
+  <si>
+    <t>public void changeSpeedAbsolute(
+int target_duty
+)
+Ähnlich wie changeSpeed, aber setzt auf target_duty statt +- direction_vector</t>
+  </si>
+  <si>
+    <t>public int steer(
+int steering_vector
+)
+wird zum lenken aufgerufen, wechselt Lenkgrad um steering_vector(Delta in %)</t>
+  </si>
+  <si>
+    <t>Anmerkung: Alle Prozentwerte haben eine Spanne von 100 bis -100 (steering_vector, direction_vector, steering_degree etc)</t>
+  </si>
+  <si>
+    <t>GitHub Repo:
+https://github.com/niklasschoening/BuggyControl</t>
+  </si>
+  <si>
     <t>SteeringServo(
 int pin, //Pin, über den dem Servo Input gegeben wird
-int power_pin, //Strom-Pin des Servos, kann NULL sein
+int power_pin, //Strom-Pin des Servos. Bei negativen Werten wird dieser nicht initiiert, falls nicht nötig
 int rest_position, //Position in Grad, bei dem der Buggy geradeaus fährt
 int max_steering_degree, //maximaler Lenkeinschlag, der möglich ist
 int deadzone //deadzone, in welchem Bereich der Servo trotzdem auf Null gesetzt wird
 )</t>
   </si>
   <si>
-    <t>public void turnOff(
-)
-schaltet alle LEDs aus</t>
-  </si>
-  <si>
-    <t>private int percentToDegree(
-int steering_percent
-)
-gibt steering_percent in Grad umgewandelt zurück</t>
-  </si>
-  <si>
-    <t>public void steeringVector(
-int steering_vector
-)
-Ändert den Lenkgrad des Buggys um steering_vector(Ähnlich wie direction_vector, Delta-Angabe in %)</t>
-  </si>
-  <si>
-    <t>public int getSteeringDegree(
-)
-Gibt aktuellen Lenkwinkeln zurück</t>
-  </si>
-  <si>
-    <t>public void changeSpeed(
-int direction_vector 
-)
-Diese Funktion sollte zum Ändern der Motorgeschwindigkeit als einzige direkt aufgerufen wird. Direction_vector ist die erwünschte Veränderung des Duty-Cycles/der Geschwindigkeit in %, kein absoluter Wert. Entscheidet anhand von threshhold, ob fadeDuty oder setDuty genutzt werden soll, initialisiert safetyDelay bei Richtungswechsel oder anhalten u.w.</t>
-  </si>
-  <si>
-    <t>public void changeSpeedAbsolute(
-int target_duty
-)
-Ähnlich wie changeSpeed, aber setzt auf target_duty statt +- direction_vector</t>
-  </si>
-  <si>
-    <t>public int steer(
-int steering_vector
-)
-wird zum lenken aufgerufen, wechselt Lenkgrad um steering_vector(Delta in %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">public int steerAbsolute(
+    <t>private int lcFunction(
+int t
+)
+gibt den Duty-Wert der Launch-Control-Kurve in Abhängigkeit von t in ms zurück</t>
+  </si>
+  <si>
+    <t>public bool stopLaunchControl(
+)
+beendet Launch-Control-Vorgang</t>
+  </si>
+  <si>
+    <t>private bool launchControl(
+)
+Funktion die während LaunchControl läuft</t>
+  </si>
+  <si>
+    <t>public void begin(
+)
+Muss aufgerufen werden, um den Servo richtig zu initialisieren</t>
+  </si>
+  <si>
+    <t>public int getSteeringPercent(
+)
+Gibt den Lenkwert in % zurück</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public void steerAbsolute(
 int steering_degree
 )
 setzt den Lenkwinkel auf steering_degree(Absoluter Lenkwinkeln in %)
 </t>
   </si>
   <si>
-    <t>Anmerkung: Alle Prozentwerte haben eine Spanne von 100 bis -100 (steering_vector, direction_vector, steering_degree etc)</t>
+    <t>public void steer(
+int steering_vector
+)
+Ändert den Lenkgrad des Buggys um steering_vector(Ähnlich wie direction_vector, Delta-Angabe in %)</t>
+  </si>
+  <si>
+    <t>public void setRestPosition(
+)
+Setzt den Servo auf Rest-Position zurück. Kann durch steerAbsolute(0) besser erreicht werden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +234,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow (Textkörper)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -279,10 +306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -305,8 +333,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCC9135-BD93-8C43-8270-F2165723A60F}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,7 +689,9 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -681,7 +715,7 @@
     <row r="4" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -692,45 +726,45 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -741,52 +775,52 @@
     </row>
     <row r="13" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -797,52 +831,76 @@
     </row>
     <row r="21" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
+    <row r="23" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+    <row r="26" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
-        <v>27</v>
+    <row r="27" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B30" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="https://github.com/niklasschoening/BuggyControl" xr:uid="{68A97D00-7691-044E-B68F-F03C016D2432}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>